<commit_message>
Add TRUE() function to the ExcelFile.xlsx
</commit_message>
<xml_diff>
--- a/src/main/java/ExcelFile.xlsx
+++ b/src/main/java/ExcelFile.xlsx
@@ -19,18 +19,11 @@
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t xml:space="preserve">Second value</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -110,7 +103,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -134,14 +127,15 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
+      <c r="A1" s="1" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>